<commit_message>
Tested live trading for kiwoom broker implementation
</commit_message>
<xml_diff>
--- a/koapy/openapi/data/fid.xlsx
+++ b/koapy/openapi/data/fid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NXZT\git\koapy\koapy\openapi\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NXZT\Documents\git\koapy\koapy\openapi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410679BC-1CDE-4A1B-B494-3D40891509AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0265BACE-6647-4ACE-B7D0-33E9CB0E23DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2310" yWindow="855" windowWidth="12585" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27585" yWindow="1785" windowWidth="20040" windowHeight="16455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2756,9 +2756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B810"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="B223" sqref="B223"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>